<commit_message>
some data for openmp-based parallel receive.
</commit_message>
<xml_diff>
--- a/direct_interface_performance.xlsx
+++ b/direct_interface_performance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kanghongbo/Desktop/PIM_at_HW/upmem_communication_performance_test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57F776D0-4A56-544A-8DDF-D4A74934CCC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE2CD80F-3E3E-3E41-8D58-EAE6CAA503FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5840" yWindow="2180" windowWidth="35080" windowHeight="23120" xr2:uid="{25B01C09-0A08-DA47-AB65-6825C89D0A76}"/>
+    <workbookView xWindow="0" yWindow="1500" windowWidth="35080" windowHeight="19240" activeTab="1" xr2:uid="{25B01C09-0A08-DA47-AB65-6825C89D0A76}"/>
   </bookViews>
   <sheets>
     <sheet name="Send" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="41">
   <si>
     <t>Direct</t>
   </si>
@@ -62,6 +62,102 @@
   </si>
   <si>
     <t>Transpose</t>
+  </si>
+  <si>
+    <t>multithread</t>
+  </si>
+  <si>
+    <t>Bandwidth</t>
+  </si>
+  <si>
+    <t>upmem</t>
+  </si>
+  <si>
+    <t>openmp+direct</t>
+  </si>
+  <si>
+    <t>4 rank</t>
+  </si>
+  <si>
+    <t>256 DPUS</t>
+  </si>
+  <si>
+    <t>1 core</t>
+  </si>
+  <si>
+    <t>Setup</t>
+  </si>
+  <si>
+    <t>2 DIMMS</t>
+  </si>
+  <si>
+    <t>2 channels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gather </t>
+  </si>
+  <si>
+    <t>Data / DPU</t>
+  </si>
+  <si>
+    <t>4 ranks</t>
+  </si>
+  <si>
+    <t>2DIMMS</t>
+  </si>
+  <si>
+    <t>1core/direct</t>
+  </si>
+  <si>
+    <t>4 threads/upmem</t>
+  </si>
+  <si>
+    <t>async send</t>
+  </si>
+  <si>
+    <t>sync</t>
+  </si>
+  <si>
+    <t>polling threads</t>
+  </si>
+  <si>
+    <t>job threads</t>
+  </si>
+  <si>
+    <t>16 ranks</t>
+  </si>
+  <si>
+    <t>8 DIMMS</t>
+  </si>
+  <si>
+    <t>? Channel</t>
+  </si>
+  <si>
+    <t>? Threads</t>
+  </si>
+  <si>
+    <t>8 cores</t>
+  </si>
+  <si>
+    <t>1024 DPUS</t>
+  </si>
+  <si>
+    <t>Total Size /KB</t>
+  </si>
+  <si>
+    <t>Size per DIMM / KB</t>
+  </si>
+  <si>
+    <t>10MB</t>
+  </si>
+  <si>
+    <t>5MB</t>
+  </si>
+  <si>
+    <t>160MB</t>
+  </si>
+  <si>
+    <t>Bandwidth Improvement</t>
   </si>
 </sst>
 </file>
@@ -886,7 +982,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Receive Speed</a:t>
+              <a:t>Receive Timespent</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1611,6 +1707,520 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Receive!$L$16</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>upmem</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Receive!$K$17:$K$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>640</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1280</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2560</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5120</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10240</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20480</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40960</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>81920</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>163840</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Receive!$L$17:$L$26</c:f>
+              <c:numCache>
+                <c:formatCode>0.000E+00</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>4.9517400000000003E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.4465799999999995E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.0486100000000005E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.3275100000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.2528999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.2813500000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.3153000000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.2325499999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.70394E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.69088E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3379-D247-90C1-143DB5EDDDC0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Receive!$M$16</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>openmp+direct</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Receive!$K$17:$K$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>640</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1280</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2560</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5120</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10240</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20480</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40960</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>81920</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>163840</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Receive!$M$17:$M$26</c:f>
+              <c:numCache>
+                <c:formatCode>0.000E+00</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>7.3958899999999994E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.3735700000000006E-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.4154400000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.0307100000000003E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.9424799999999996E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.5307400000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.3904600000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.8428300000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.1571699999999992E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.6890500000000001E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-3379-D247-90C1-143DB5EDDDC0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="938787104"/>
+        <c:axId val="939035984"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="938787104"/>
+        <c:scaling>
+          <c:logBase val="2"/>
+          <c:orientation val="minMax"/>
+          <c:min val="320"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="939035984"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="939035984"/>
+        <c:scaling>
+          <c:logBase val="2"/>
+          <c:orientation val="minMax"/>
+          <c:max val="0.05"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.000E+00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="938787104"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1691,6 +2301,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -2208,6 +2858,522 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2770,16 +3936,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>12624</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>113780</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>5197</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>2377</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>432987</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>49612</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>759771</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>138734</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2799,6 +3965,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>689093</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>176702</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>863130</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>66321</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1305BAE2-D038-98F8-3085-87711107B38E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3104,19 +4306,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC65E1C-CFD6-4D4D-8153-31217B9DE945}">
-  <dimension ref="B2:L12"/>
+  <dimension ref="B1:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="171" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView topLeftCell="A9" zoomScale="171" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="5" max="5" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.6640625" customWidth="1"/>
-    <col min="8" max="8" width="12.33203125" customWidth="1"/>
+    <col min="7" max="7" width="16.83203125" customWidth="1"/>
+    <col min="8" max="8" width="14.83203125" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" t="s">
+        <v>24</v>
+      </c>
+    </row>
     <row r="2" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>2</v>
@@ -3163,7 +4385,10 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
+      <c r="K3" s="2">
+        <f>B3/D3/1024/1024/1024</f>
+        <v>0.17919472311278656</v>
+      </c>
       <c r="L3" s="2"/>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.2">
@@ -3183,7 +4408,10 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
+      <c r="K4" s="2">
+        <f t="shared" ref="K4:K12" si="1">B4/D4/1024/1024/1024</f>
+        <v>0.48343146553772559</v>
+      </c>
       <c r="L4" s="2"/>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.2">
@@ -3203,7 +4431,10 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
+      <c r="K5" s="2">
+        <f t="shared" si="1"/>
+        <v>0.80853582002556679</v>
+      </c>
       <c r="L5" s="2"/>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.2">
@@ -3223,7 +4454,10 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
+      <c r="K6" s="2">
+        <f t="shared" si="1"/>
+        <v>1.3884801203414605</v>
+      </c>
       <c r="L6" s="2"/>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.2">
@@ -3241,7 +4475,10 @@
       <c r="F7" s="2"/>
       <c r="G7" s="1"/>
       <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
+      <c r="K7" s="2">
+        <f t="shared" si="1"/>
+        <v>2.7528809670126457</v>
+      </c>
       <c r="L7" s="2"/>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.2">
@@ -3259,7 +4496,10 @@
       <c r="F8" s="2"/>
       <c r="G8" s="1"/>
       <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
+      <c r="K8" s="2">
+        <f t="shared" si="1"/>
+        <v>3.8550853077949458</v>
+      </c>
       <c r="L8" s="2"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.2">
@@ -3277,7 +4517,10 @@
       <c r="F9" s="2"/>
       <c r="G9" s="1"/>
       <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
+      <c r="K9" s="2">
+        <f t="shared" si="1"/>
+        <v>4.7993163930518801</v>
+      </c>
       <c r="L9" s="2"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.2">
@@ -3294,7 +4537,10 @@
       <c r="E10" s="1"/>
       <c r="F10" s="2"/>
       <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
+      <c r="K10" s="2">
+        <f t="shared" si="1"/>
+        <v>5.3958573628847892</v>
+      </c>
       <c r="L10" s="2"/>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.2">
@@ -3311,7 +4557,10 @@
       <c r="E11" s="1"/>
       <c r="F11" s="2"/>
       <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
+      <c r="K11" s="2">
+        <f t="shared" si="1"/>
+        <v>5.7800153887129708</v>
+      </c>
       <c r="L11" s="2"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.2">
@@ -3328,8 +4577,27 @@
       <c r="E12" s="1"/>
       <c r="F12" s="2"/>
       <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
+      <c r="K12" s="2">
+        <f t="shared" si="1"/>
+        <v>6.3383309805448729</v>
+      </c>
       <c r="L12" s="2"/>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="G14" t="s">
+        <v>25</v>
+      </c>
+      <c r="H14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="G15" t="s">
+        <v>28</v>
+      </c>
+      <c r="H15" t="s">
+        <v>27</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3339,10 +4607,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDFA6D14-5D50-4742-B282-3D26B3553ED8}">
-  <dimension ref="B2:L12"/>
+  <dimension ref="A1:P26"/>
   <sheetViews>
-    <sheetView zoomScale="171" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView tabSelected="1" zoomScale="133" workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3350,9 +4618,38 @@
     <col min="5" max="5" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.6640625" customWidth="1"/>
     <col min="8" max="8" width="12.33203125" customWidth="1"/>
+    <col min="13" max="13" width="14.5" customWidth="1"/>
+    <col min="15" max="15" width="14.5" customWidth="1"/>
+    <col min="16" max="16" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
@@ -3381,7 +4678,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <f>B3/256</f>
+        <v>128</v>
+      </c>
       <c r="B3">
         <v>32768</v>
       </c>
@@ -3410,13 +4711,12 @@
       <c r="J3" s="2">
         <v>2.2651200000000001E-5</v>
       </c>
-      <c r="K3" s="2">
-        <f>B3/J3/1048576/1024</f>
-        <v>1.347283063369711</v>
-      </c>
-      <c r="L3" s="2"/>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <f t="shared" ref="A4:A12" si="1">B4/256</f>
+        <v>256</v>
+      </c>
       <c r="B4">
         <v>65536</v>
       </c>
@@ -3445,13 +4745,12 @@
       <c r="J4" s="2">
         <v>3.4699700000000003E-5</v>
       </c>
-      <c r="K4" s="2">
-        <f t="shared" ref="K4:K12" si="1">B4/J4/1048576/1024</f>
-        <v>1.7589534275512466</v>
-      </c>
-      <c r="L4" s="2"/>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <f t="shared" si="1"/>
+        <v>512</v>
+      </c>
       <c r="B5">
         <v>131072</v>
       </c>
@@ -3480,13 +4779,12 @@
       <c r="J5" s="2">
         <v>6.2198400000000004E-5</v>
       </c>
-      <c r="K5" s="2">
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A6">
         <f t="shared" si="1"/>
-        <v>1.9625957018186961</v>
-      </c>
-      <c r="L5" s="2"/>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.2">
+        <v>1024</v>
+      </c>
       <c r="B6">
         <v>262144</v>
       </c>
@@ -3515,13 +4813,12 @@
       <c r="J6" s="2">
         <v>1.17137E-4</v>
       </c>
-      <c r="K6" s="2">
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A7">
         <f t="shared" si="1"/>
-        <v>2.0842314981602739</v>
-      </c>
-      <c r="L6" s="2"/>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.2">
+        <v>2048</v>
+      </c>
       <c r="B7">
         <v>524288</v>
       </c>
@@ -3550,13 +4847,12 @@
       <c r="J7" s="2">
         <v>2.23465E-4</v>
       </c>
-      <c r="K7" s="2">
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A8">
         <f t="shared" si="1"/>
-        <v>2.1850457566061801</v>
-      </c>
-      <c r="L7" s="2"/>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.2">
+        <v>4096</v>
+      </c>
       <c r="B8">
         <v>1048576</v>
       </c>
@@ -3585,13 +4881,12 @@
       <c r="J8" s="2">
         <v>4.6504000000000001E-4</v>
       </c>
-      <c r="K8" s="2">
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A9">
         <f t="shared" si="1"/>
-        <v>2.0999537674178566</v>
-      </c>
-      <c r="L8" s="2"/>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.2">
+        <v>8192</v>
+      </c>
       <c r="B9">
         <v>2097152</v>
       </c>
@@ -3620,13 +4915,12 @@
       <c r="J9" s="2">
         <v>8.0728799999999997E-4</v>
       </c>
-      <c r="K9" s="2">
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A10">
         <f t="shared" si="1"/>
-        <v>2.4193658273131771</v>
-      </c>
-      <c r="L9" s="2"/>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.2">
+        <v>16384</v>
+      </c>
       <c r="B10">
         <v>4194304</v>
       </c>
@@ -3655,13 +4949,12 @@
       <c r="J10" s="2">
         <v>1.5742600000000001E-3</v>
       </c>
-      <c r="K10" s="2">
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A11">
         <f t="shared" si="1"/>
-        <v>2.4813245588403441</v>
-      </c>
-      <c r="L10" s="2"/>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.2">
+        <v>32768</v>
+      </c>
       <c r="B11">
         <v>8388608</v>
       </c>
@@ -3690,13 +4983,12 @@
       <c r="J11" s="2">
         <v>3.1707100000000002E-3</v>
       </c>
-      <c r="K11" s="2">
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A12">
         <f t="shared" si="1"/>
-        <v>2.4639591763358992</v>
-      </c>
-      <c r="L11" s="2"/>
-    </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.2">
+        <v>65536</v>
+      </c>
       <c r="B12">
         <v>16777216</v>
       </c>
@@ -3725,11 +5017,300 @@
       <c r="J12" s="2">
         <v>6.4426500000000003E-3</v>
       </c>
-      <c r="K12" s="2">
-        <f t="shared" si="1"/>
-        <v>2.4252442706029349</v>
-      </c>
-      <c r="L12" s="2"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="L14" t="s">
+        <v>32</v>
+      </c>
+      <c r="M14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="L15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M15" t="s">
+        <v>29</v>
+      </c>
+      <c r="N15" t="s">
+        <v>30</v>
+      </c>
+      <c r="O15" t="s">
+        <v>31</v>
+      </c>
+      <c r="P15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="K16" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L16" t="s">
+        <v>11</v>
+      </c>
+      <c r="M16" t="s">
+        <v>12</v>
+      </c>
+      <c r="N16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="O16" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="P16" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="10:16" x14ac:dyDescent="0.2">
+      <c r="K17">
+        <f>B3*10/1024</f>
+        <v>320</v>
+      </c>
+      <c r="L17" s="2">
+        <v>4.9517400000000003E-4</v>
+      </c>
+      <c r="M17" s="2">
+        <v>7.3958899999999994E-5</v>
+      </c>
+      <c r="N17" s="2">
+        <f>B3/M17/1024/1024/1024*10</f>
+        <v>4.1262888070266062</v>
+      </c>
+      <c r="O17">
+        <f>K17/16/64</f>
+        <v>0.3125</v>
+      </c>
+      <c r="P17" s="2">
+        <f>L17/M17</f>
+        <v>6.6952591236484054</v>
+      </c>
+    </row>
+    <row r="18" spans="10:16" x14ac:dyDescent="0.2">
+      <c r="K18">
+        <f>B4*10/1024</f>
+        <v>640</v>
+      </c>
+      <c r="L18" s="2">
+        <v>5.4465799999999995E-4</v>
+      </c>
+      <c r="M18" s="2">
+        <v>7.3735700000000006E-5</v>
+      </c>
+      <c r="N18" s="2">
+        <f>B4/M18/1024/1024/1024*10</f>
+        <v>8.2775583943734166</v>
+      </c>
+      <c r="O18">
+        <f>K18/16/64</f>
+        <v>0.625</v>
+      </c>
+      <c r="P18" s="2">
+        <f>L18/M18</f>
+        <v>7.3866254744987829</v>
+      </c>
+    </row>
+    <row r="19" spans="10:16" x14ac:dyDescent="0.2">
+      <c r="K19">
+        <f>B5*10/1024</f>
+        <v>1280</v>
+      </c>
+      <c r="L19" s="2">
+        <v>6.0486100000000005E-4</v>
+      </c>
+      <c r="M19" s="2">
+        <v>1.4154400000000001E-4</v>
+      </c>
+      <c r="N19" s="2">
+        <f>B5/M19/1024/1024/1024*10</f>
+        <v>8.6241954798507887</v>
+      </c>
+      <c r="O19">
+        <f>K19/16/64</f>
+        <v>1.25</v>
+      </c>
+      <c r="P19" s="2">
+        <f>L19/M19</f>
+        <v>4.273307240151472</v>
+      </c>
+    </row>
+    <row r="20" spans="10:16" x14ac:dyDescent="0.2">
+      <c r="K20">
+        <f>B6*10/1024</f>
+        <v>2560</v>
+      </c>
+      <c r="L20" s="2">
+        <v>7.3275100000000002E-4</v>
+      </c>
+      <c r="M20" s="2">
+        <v>3.0307100000000003E-4</v>
+      </c>
+      <c r="N20" s="2">
+        <f>B6/M20/1024/1024/1024*10</f>
+        <v>8.0555587634580679</v>
+      </c>
+      <c r="O20">
+        <f>K20/16/64</f>
+        <v>2.5</v>
+      </c>
+      <c r="P20" s="2">
+        <f>L20/M20</f>
+        <v>2.4177535956920986</v>
+      </c>
+    </row>
+    <row r="21" spans="10:16" x14ac:dyDescent="0.2">
+      <c r="J21" t="s">
+        <v>38</v>
+      </c>
+      <c r="K21">
+        <f>B7*10/1024</f>
+        <v>5120</v>
+      </c>
+      <c r="L21" s="2">
+        <v>1.2528999999999999E-3</v>
+      </c>
+      <c r="M21" s="2">
+        <v>6.9424799999999996E-4</v>
+      </c>
+      <c r="N21" s="2">
+        <f>B7/M21/1024/1024/1024*10</f>
+        <v>7.0332395628075268</v>
+      </c>
+      <c r="O21">
+        <f>K21/16/64</f>
+        <v>5</v>
+      </c>
+      <c r="P21" s="2">
+        <f>L21/M21</f>
+        <v>1.8046865097198697</v>
+      </c>
+    </row>
+    <row r="22" spans="10:16" x14ac:dyDescent="0.2">
+      <c r="J22" t="s">
+        <v>37</v>
+      </c>
+      <c r="K22">
+        <f>B8*10/1024</f>
+        <v>10240</v>
+      </c>
+      <c r="L22" s="2">
+        <v>2.2813500000000001E-3</v>
+      </c>
+      <c r="M22" s="2">
+        <v>1.5307400000000001E-3</v>
+      </c>
+      <c r="N22" s="2">
+        <f>B8/M22/1024/1024/1024*10</f>
+        <v>6.3796758430562992</v>
+      </c>
+      <c r="O22">
+        <f>K22/16/64</f>
+        <v>10</v>
+      </c>
+      <c r="P22" s="2">
+        <f>L22/M22</f>
+        <v>1.4903576048185845</v>
+      </c>
+    </row>
+    <row r="23" spans="10:16" x14ac:dyDescent="0.2">
+      <c r="K23">
+        <f>B9*10/1024</f>
+        <v>20480</v>
+      </c>
+      <c r="L23" s="2">
+        <v>4.3153000000000002E-3</v>
+      </c>
+      <c r="M23" s="2">
+        <v>2.3904600000000001E-3</v>
+      </c>
+      <c r="N23" s="2">
+        <f>B9/M23/1024/1024/1024*10</f>
+        <v>8.1704985651297228</v>
+      </c>
+      <c r="O23">
+        <f>K23/16/64</f>
+        <v>20</v>
+      </c>
+      <c r="P23" s="2">
+        <f>L23/M23</f>
+        <v>1.8052174058549402</v>
+      </c>
+    </row>
+    <row r="24" spans="10:16" x14ac:dyDescent="0.2">
+      <c r="K24">
+        <f>B10*10/1024</f>
+        <v>40960</v>
+      </c>
+      <c r="L24" s="2">
+        <v>8.2325499999999999E-3</v>
+      </c>
+      <c r="M24" s="2">
+        <v>4.8428300000000002E-3</v>
+      </c>
+      <c r="N24" s="2">
+        <f>B10/M24/1024/1024/1024*10</f>
+        <v>8.066048157792034</v>
+      </c>
+      <c r="O24">
+        <f>K24/16/64</f>
+        <v>40</v>
+      </c>
+      <c r="P24" s="2">
+        <f>L24/M24</f>
+        <v>1.6999461058926288</v>
+      </c>
+    </row>
+    <row r="25" spans="10:16" x14ac:dyDescent="0.2">
+      <c r="K25">
+        <f>B11*10/1024</f>
+        <v>81920</v>
+      </c>
+      <c r="L25" s="2">
+        <v>1.70394E-2</v>
+      </c>
+      <c r="M25" s="2">
+        <v>9.1571699999999992E-3</v>
+      </c>
+      <c r="N25" s="2">
+        <f>B11/M25/1024/1024/1024*10</f>
+        <v>8.531565975077454</v>
+      </c>
+      <c r="O25">
+        <f>K25/16/64</f>
+        <v>80</v>
+      </c>
+      <c r="P25" s="2">
+        <f>L25/M25</f>
+        <v>1.860771395529405</v>
+      </c>
+    </row>
+    <row r="26" spans="10:16" x14ac:dyDescent="0.2">
+      <c r="J26" t="s">
+        <v>39</v>
+      </c>
+      <c r="K26">
+        <f>B12*10/1024</f>
+        <v>163840</v>
+      </c>
+      <c r="L26" s="2">
+        <v>2.69088E-2</v>
+      </c>
+      <c r="M26" s="2">
+        <v>2.6890500000000001E-2</v>
+      </c>
+      <c r="N26" s="2">
+        <f>B12/M26/1024/1024/1024*10</f>
+        <v>5.8106022573027651</v>
+      </c>
+      <c r="O26">
+        <f>K26/16/64</f>
+        <v>160</v>
+      </c>
+      <c r="P26" s="2">
+        <f>L26/M26</f>
+        <v>1.0006805377363752</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
send supported. probably dangerous. additional protection added.
</commit_message>
<xml_diff>
--- a/direct_interface_performance.xlsx
+++ b/direct_interface_performance.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kanghongbo/Desktop/PIM_at_HW/upmem_communication_performance_test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE2CD80F-3E3E-3E41-8D58-EAE6CAA503FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{262AF9B3-FA59-5F49-871B-F655CCB1DA43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1500" windowWidth="35080" windowHeight="19240" activeTab="1" xr2:uid="{25B01C09-0A08-DA47-AB65-6825C89D0A76}"/>
+    <workbookView xWindow="5560" yWindow="6860" windowWidth="35080" windowHeight="19240" activeTab="1" xr2:uid="{25B01C09-0A08-DA47-AB65-6825C89D0A76}"/>
   </bookViews>
   <sheets>
     <sheet name="Send" sheetId="2" r:id="rId1"/>
-    <sheet name="Receive" sheetId="1" r:id="rId2"/>
+    <sheet name="Receive" sheetId="3" r:id="rId2"/>
+    <sheet name="ReceiveDev" sheetId="1" r:id="rId3"/>
+    <sheet name="Launch" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="56">
   <si>
     <t>Direct</t>
   </si>
@@ -112,18 +114,6 @@
     <t>4 threads/upmem</t>
   </si>
   <si>
-    <t>async send</t>
-  </si>
-  <si>
-    <t>sync</t>
-  </si>
-  <si>
-    <t>polling threads</t>
-  </si>
-  <si>
-    <t>job threads</t>
-  </si>
-  <si>
     <t>16 ranks</t>
   </si>
   <si>
@@ -159,6 +149,63 @@
   <si>
     <t>Bandwidth Improvement</t>
   </si>
+  <si>
+    <t>{"buffer_length":256,"mode":"sync","offset":0,"total_length":65536,"type":"send"}</t>
+  </si>
+  <si>
+    <t>{"buffer_length":256,"mode":"sync","offset":256,"total_length":65536,"type":"receive"}</t>
+  </si>
+  <si>
+    <t>{"type":"exec"}</t>
+  </si>
+  <si>
+    <t>{"buffer_length":256,"mode":"sync","offset":512,"total_length":65536,"type":"receive"}</t>
+  </si>
+  <si>
+    <t>{"buffer_length":256,"mode":"sync","offset":768,"total_length":65536,"type":"receive"}</t>
+  </si>
+  <si>
+    <t>Ownership of memory</t>
+  </si>
+  <si>
+    <t>host</t>
+  </si>
+  <si>
+    <t>host-&gt;DPU</t>
+  </si>
+  <si>
+    <t>DPU-&gt;host</t>
+  </si>
+  <si>
+    <t>Common</t>
+  </si>
+  <si>
+    <t>on 2 DIMMS</t>
+  </si>
+  <si>
+    <t>on 2 channels</t>
+  </si>
+  <si>
+    <t>4 ranks = 256 DPUS</t>
+  </si>
+  <si>
+    <t>UPMEM SDK</t>
+  </si>
+  <si>
+    <t>&gt;4 threads on &gt;4 cores</t>
+  </si>
+  <si>
+    <t>Ideal</t>
+  </si>
+  <si>
+    <t>assume 10ns / cacheline</t>
+  </si>
+  <si>
+    <t>1 thread on 1 core</t>
+  </si>
+  <si>
+    <t>actual # threads unclear because of UPMEM SDK's implementation</t>
+  </si>
 </sst>
 </file>
 
@@ -167,7 +214,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000E+00"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -175,13 +222,49 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -193,15 +276,29 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="0" xfId="3" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -385,33 +482,39 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>32768</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
                   <c:v>65536</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>131072</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>262144</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>524288</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>1048576</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>2097152</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>4194304</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>8388608</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>16777216</c:v>
                 </c:pt>
               </c:numCache>
@@ -424,33 +527,39 @@
                 <c:formatCode>0.000E+00</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
+                  <c:v>1.28E-6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.5600000000000001E-6</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>5.1200000000000001E-6</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
                   <c:v>1.024E-5</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>2.048E-5</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>4.0960000000000001E-5</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>8.1920000000000002E-5</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>1.6384E-4</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>3.2768000000000001E-4</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>6.5536000000000001E-4</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>1.31072E-3</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>2.6214400000000001E-3</c:v>
                 </c:pt>
               </c:numCache>
@@ -506,33 +615,39 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>32768</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
                   <c:v>65536</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>131072</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>262144</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>524288</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>1048576</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>2097152</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>4194304</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>8388608</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>16777216</c:v>
                 </c:pt>
               </c:numCache>
@@ -542,37 +657,43 @@
             <c:numRef>
               <c:f>Send!$D$3:$D$15</c:f>
               <c:numCache>
-                <c:formatCode>0.000E+00</c:formatCode>
+                <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="13"/>
-                <c:pt idx="0">
-                  <c:v>1.70304E-4</c:v>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>1.4195399999999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.2625399999999999E-4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.50977E-4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.75833E-4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.7737100000000001E-4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.5331799999999999E-4</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>4.0695899999999998E-4</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7.2393499999999999E-4</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.3516400000000001E-3</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2.4651600000000001E-3</c:v>
+                  <c:v>9.6364299999999995E-5</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="0.000E+00">
+                  <c:v>9.9926000000000005E-5</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0.000E+00">
+                  <c:v>1.14082E-4</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.000E+00">
+                  <c:v>1.4262300000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0.000E+00">
+                  <c:v>1.6004699999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="0.000E+00">
+                  <c:v>1.65599E-4</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="0.000E+00">
+                  <c:v>2.34305E-4</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="0.000E+00">
+                  <c:v>3.9397500000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="0.000E+00">
+                  <c:v>6.9665500000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="0.000E+00">
+                  <c:v>1.2886200000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="0.000E+00">
+                  <c:v>2.3513900000000001E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -677,33 +798,39 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>32768</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
                   <c:v>65536</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>131072</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>262144</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>524288</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>1048576</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>2097152</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>4194304</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>8388608</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>16777216</c:v>
                 </c:pt>
               </c:numCache>
@@ -711,10 +838,46 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Send!$J$3:$J$12</c:f>
+              <c:f>Send!$J$3:$J$14</c:f>
               <c:numCache>
-                <c:formatCode>0.000E+00</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1.0166899999999999E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.99869E-5</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="0.000E+00">
+                  <c:v>1.6050599999999998E-5</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0.000E+00">
+                  <c:v>2.5599700000000002E-5</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.000E+00">
+                  <c:v>5.1776200000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0.000E+00">
+                  <c:v>9.9921199999999995E-5</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="0.000E+00">
+                  <c:v>2.0879899999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="0.000E+00">
+                  <c:v>3.8256400000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="0.000E+00">
+                  <c:v>7.1241200000000005E-4</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="0.000E+00">
+                  <c:v>1.35732E-3</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="0.000E+00">
+                  <c:v>2.6243400000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="0.000E+00">
+                  <c:v>5.6999700000000004E-3</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -741,7 +904,7 @@
         <c:scaling>
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
-          <c:min val="32768"/>
+          <c:min val="8192"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -982,7 +1145,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Receive Timespent</a:t>
+              <a:t>Receive Speed</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1115,33 +1278,39 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>32768</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
                   <c:v>65536</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>131072</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>262144</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>524288</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>1048576</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>2097152</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>4194304</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>8388608</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>16777216</c:v>
                 </c:pt>
               </c:numCache>
@@ -1154,33 +1323,39 @@
                 <c:formatCode>0.000E+00</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
+                  <c:v>1.28E-6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.5600000000000001E-6</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>5.1200000000000001E-6</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
                   <c:v>1.024E-5</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>2.048E-5</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>4.0960000000000001E-5</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>8.1920000000000002E-5</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>1.6384E-4</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>3.2768000000000001E-4</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>6.5536000000000001E-4</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>1.31072E-3</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>2.6214400000000001E-3</c:v>
                 </c:pt>
               </c:numCache>
@@ -1189,7 +1364,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-7222-EB42-B75A-0AC4A1CD3C25}"/>
+              <c16:uniqueId val="{00000001-345B-AF4D-AB16-3E1D666B96FF}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1236,33 +1411,39 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>32768</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
                   <c:v>65536</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>131072</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>262144</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>524288</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>1048576</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>2097152</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>4194304</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>8388608</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>16777216</c:v>
                 </c:pt>
               </c:numCache>
@@ -1272,37 +1453,43 @@
             <c:numRef>
               <c:f>Receive!$D$3:$D$15</c:f>
               <c:numCache>
-                <c:formatCode>0.000E+00</c:formatCode>
+                <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="13"/>
-                <c:pt idx="0">
-                  <c:v>1.7191099999999999E-4</c:v>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>1.42118E-4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.51664E-4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.0755E-4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2.1600300000000001E-4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2.1555399999999999E-4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3.2564699999999998E-4</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>5.6045499999999996E-4</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.04116E-3</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2.0522000000000001E-3</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>3.9906300000000002E-3</c:v>
+                  <c:v>1.04782E-4</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="0.000E+00">
+                  <c:v>1.17465E-4</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0.000E+00">
+                  <c:v>1.4510400000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.000E+00">
+                  <c:v>2.0185900000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0.000E+00">
+                  <c:v>2.1001900000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="0.000E+00">
+                  <c:v>2.2035499999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="0.000E+00">
+                  <c:v>3.2559499999999998E-4</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="0.000E+00">
+                  <c:v>5.6724200000000003E-4</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="0.000E+00">
+                  <c:v>1.0412799999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="0.000E+00">
+                  <c:v>2.0467100000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="0.000E+00">
+                  <c:v>4.01798E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1310,7 +1497,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-7222-EB42-B75A-0AC4A1CD3C25}"/>
+              <c16:uniqueId val="{00000002-345B-AF4D-AB16-3E1D666B96FF}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1407,33 +1594,39 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>32768</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
                   <c:v>65536</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>131072</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>262144</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>524288</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>1048576</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>2097152</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>4194304</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>8388608</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>16777216</c:v>
                 </c:pt>
               </c:numCache>
@@ -1441,7 +1634,773 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Receive!$J$3:$J$12</c:f>
+              <c:f>Receive!$J$3:$J$14</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1.29774E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.5007E-5</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="0.000E+00">
+                  <c:v>2.0780300000000002E-5</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0.000E+00">
+                  <c:v>3.5589700000000002E-5</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.000E+00">
+                  <c:v>6.3728799999999999E-5</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0.000E+00">
+                  <c:v>1.1654099999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="0.000E+00">
+                  <c:v>2.2104000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="0.000E+00">
+                  <c:v>4.3998099999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="0.000E+00">
+                  <c:v>8.5231300000000005E-4</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="0.000E+00">
+                  <c:v>1.6706799999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="0.000E+00">
+                  <c:v>3.45809E-3</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="0.000E+00">
+                  <c:v>6.8170100000000001E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-345B-AF4D-AB16-3E1D666B96FF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1443279216"/>
+        <c:axId val="1443251776"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1443279216"/>
+        <c:scaling>
+          <c:logBase val="2"/>
+          <c:orientation val="minMax"/>
+          <c:min val="8192"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1443251776"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1443251776"/>
+        <c:scaling>
+          <c:logBase val="2"/>
+          <c:orientation val="minMax"/>
+          <c:max val="0.01"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.000E+00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1443279216"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Receive Timespent</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>ReceiveDev!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>IDEAL</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.6125109361329835E-2"/>
+                  <c:y val="0.16396252551764362"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="0.00E+00" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-CN"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>ReceiveDev!$B$3:$B$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>32768</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>65536</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>131072</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>262144</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>524288</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1048576</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2097152</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4194304</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8388608</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>16777216</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>ReceiveDev!$C$3:$C$15</c:f>
+              <c:numCache>
+                <c:formatCode>0.000E+00</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>5.1200000000000001E-6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.024E-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.048E-5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0960000000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.1920000000000002E-5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.6384E-4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.2768000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.5536000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.31072E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.6214400000000001E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7222-EB42-B75A-0AC4A1CD3C25}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>ReceiveDev!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>UPMEM</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>ReceiveDev!$B$3:$B$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>32768</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>65536</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>131072</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>262144</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>524288</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1048576</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2097152</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4194304</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8388608</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>16777216</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>ReceiveDev!$D$3:$D$15</c:f>
+              <c:numCache>
+                <c:formatCode>0.000E+00</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>1.7191099999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.51664E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0755E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.1600300000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.1555399999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.2564699999999998E-4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.6045499999999996E-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.04116E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.0522000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.9906300000000002E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-7222-EB42-B75A-0AC4A1CD3C25}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>ReceiveDev!$J$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Direct</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.26289594964423668"/>
+                  <c:y val="3.1990740740740743E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="0.00E+00" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-CN"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>ReceiveDev!$B$3:$B$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>32768</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>65536</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>131072</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>262144</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>524288</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1048576</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2097152</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4194304</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8388608</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>16777216</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>ReceiveDev!$J$3:$J$12</c:f>
               <c:numCache>
                 <c:formatCode>0.000E+00</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1707,7 +2666,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1762,7 +2721,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Receive!$L$16</c:f>
+              <c:f>ReceiveDev!$L$16</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1795,7 +2754,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Receive!$K$17:$K$26</c:f>
+              <c:f>ReceiveDev!$K$17:$K$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1834,7 +2793,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Receive!$L$17:$L$26</c:f>
+              <c:f>ReceiveDev!$L$17:$L$26</c:f>
               <c:numCache>
                 <c:formatCode>0.000E+00</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1883,7 +2842,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Receive!$M$16</c:f>
+              <c:f>ReceiveDev!$M$16</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1916,7 +2875,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Receive!$K$17:$K$26</c:f>
+              <c:f>ReceiveDev!$K$17:$K$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1955,7 +2914,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Receive!$M$17:$M$26</c:f>
+              <c:f>ReceiveDev!$M$17:$M$26</c:f>
               <c:numCache>
                 <c:formatCode>0.000E+00</c:formatCode>
                 <c:ptCount val="10"/>
@@ -2341,6 +3300,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -3889,20 +4888,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>12624</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>113780</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>718179</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>96141</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>432987</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>49612</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>327153</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>31972</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3933,6 +5448,49 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>63424</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>135289</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>483787</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>71121</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A684912-3265-3C41-BE4E-57300F6B48E1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -4306,40 +5864,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC65E1C-CFD6-4D4D-8153-31217B9DE945}">
-  <dimension ref="B1:L15"/>
+  <dimension ref="A2:L19"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="171" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView zoomScale="144" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="2" max="2" width="18.33203125" customWidth="1"/>
+    <col min="3" max="3" width="24.33203125" customWidth="1"/>
+    <col min="4" max="4" width="23.83203125" customWidth="1"/>
     <col min="5" max="5" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.83203125" customWidth="1"/>
     <col min="8" max="8" width="14.83203125" customWidth="1"/>
+    <col min="10" max="10" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
@@ -4368,235 +5910,322 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B3">
+    <row r="3" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="3">
+        <v>8192</v>
+      </c>
+      <c r="C3" s="4">
+        <f t="shared" ref="C3:C4" si="0">B3/64*10/1000000000</f>
+        <v>1.28E-6</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1.4195399999999999E-4</v>
+      </c>
+      <c r="J3" s="5">
+        <v>1.0166899999999999E-5</v>
+      </c>
+      <c r="K3" s="4">
+        <f>D3/J3</f>
+        <v>13.962368076798237</v>
+      </c>
+      <c r="L3" s="4"/>
+    </row>
+    <row r="4" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="3">
+        <v>16384</v>
+      </c>
+      <c r="C4" s="4">
+        <f t="shared" si="0"/>
+        <v>2.5600000000000001E-6</v>
+      </c>
+      <c r="D4" s="5">
+        <v>9.6364299999999995E-5</v>
+      </c>
+      <c r="J4" s="5">
+        <v>1.99869E-5</v>
+      </c>
+      <c r="K4" s="4">
+        <f>D4/J4</f>
+        <v>4.8213729993145504</v>
+      </c>
+      <c r="L4" s="4"/>
+    </row>
+    <row r="5" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="3">
         <v>32768</v>
       </c>
-      <c r="C3" s="2">
-        <f t="shared" ref="C3:C12" si="0">B3/64*10/1000000000</f>
+      <c r="C5" s="4">
+        <f t="shared" ref="C5:C14" si="1">B5/64*10/1000000000</f>
         <v>5.1200000000000001E-6</v>
       </c>
-      <c r="D3" s="2">
-        <v>1.70304E-4</v>
-      </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2">
-        <f>B3/D3/1024/1024/1024</f>
-        <v>0.17919472311278656</v>
-      </c>
-      <c r="L3" s="2"/>
+      <c r="D5" s="4">
+        <v>9.9926000000000005E-5</v>
+      </c>
+      <c r="E5" s="5"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="4">
+        <v>1.6050599999999998E-5</v>
+      </c>
+      <c r="K5" s="4">
+        <f>D5/J5</f>
+        <v>6.2256862671800439</v>
+      </c>
+      <c r="L5" s="4"/>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B4">
+    <row r="6" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="3">
         <v>65536</v>
       </c>
-      <c r="C4" s="2">
-        <f t="shared" si="0"/>
+      <c r="C6" s="4">
+        <f t="shared" si="1"/>
         <v>1.024E-5</v>
       </c>
-      <c r="D4" s="2">
-        <v>1.2625399999999999E-4</v>
-      </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2">
-        <f t="shared" ref="K4:K12" si="1">B4/D4/1024/1024/1024</f>
-        <v>0.48343146553772559</v>
-      </c>
-      <c r="L4" s="2"/>
+      <c r="D6" s="4">
+        <v>1.14082E-4</v>
+      </c>
+      <c r="E6" s="5"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="4">
+        <v>2.5599700000000002E-5</v>
+      </c>
+      <c r="K6" s="4">
+        <f t="shared" ref="K6:K14" si="2">D6/J6</f>
+        <v>4.4563803482072055</v>
+      </c>
+      <c r="L6" s="4"/>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B5">
+    <row r="7" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="3">
         <v>131072</v>
       </c>
-      <c r="C5" s="2">
-        <f t="shared" si="0"/>
+      <c r="C7" s="4">
+        <f t="shared" si="1"/>
         <v>2.048E-5</v>
       </c>
-      <c r="D5" s="2">
-        <v>1.50977E-4</v>
-      </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2">
+      <c r="D7" s="4">
+        <v>1.4262300000000001E-4</v>
+      </c>
+      <c r="E7" s="5"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="4">
+        <v>5.1776200000000001E-5</v>
+      </c>
+      <c r="K7" s="4">
+        <f t="shared" si="2"/>
+        <v>2.7546053978468872</v>
+      </c>
+      <c r="L7" s="4"/>
+    </row>
+    <row r="8" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="3">
+        <f>B8/256</f>
+        <v>1024</v>
+      </c>
+      <c r="B8" s="3">
+        <v>262144</v>
+      </c>
+      <c r="C8" s="4">
         <f t="shared" si="1"/>
-        <v>0.80853582002556679</v>
-      </c>
-      <c r="L5" s="2"/>
+        <v>4.0960000000000001E-5</v>
+      </c>
+      <c r="D8" s="4">
+        <v>1.6004699999999999E-4</v>
+      </c>
+      <c r="E8" s="5"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="4">
+        <v>9.9921199999999995E-5</v>
+      </c>
+      <c r="K8" s="4">
+        <f t="shared" si="2"/>
+        <v>1.6017321649459775</v>
+      </c>
+      <c r="L8" s="4"/>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B6">
-        <v>262144</v>
-      </c>
-      <c r="C6" s="2">
-        <f t="shared" si="0"/>
-        <v>4.0960000000000001E-5</v>
-      </c>
-      <c r="D6" s="2">
-        <v>1.75833E-4</v>
-      </c>
-      <c r="E6" s="1"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2">
+    <row r="9" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="6">
+        <v>524288</v>
+      </c>
+      <c r="C9" s="7">
         <f t="shared" si="1"/>
-        <v>1.3884801203414605</v>
-      </c>
-      <c r="L6" s="2"/>
+        <v>8.1920000000000002E-5</v>
+      </c>
+      <c r="D9" s="7">
+        <v>1.65599E-4</v>
+      </c>
+      <c r="E9" s="8"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="8"/>
+      <c r="J9" s="7">
+        <v>2.0879899999999999E-4</v>
+      </c>
+      <c r="K9" s="7">
+        <f t="shared" si="2"/>
+        <v>0.79310245738724805</v>
+      </c>
+      <c r="L9" s="7"/>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B7">
-        <v>524288</v>
-      </c>
-      <c r="C7" s="2">
-        <f t="shared" si="0"/>
-        <v>8.1920000000000002E-5</v>
-      </c>
-      <c r="D7" s="2">
-        <v>1.7737100000000001E-4</v>
-      </c>
-      <c r="E7" s="1"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="1"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2">
+    <row r="10" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="6">
+        <v>1048576</v>
+      </c>
+      <c r="C10" s="7">
         <f t="shared" si="1"/>
-        <v>2.7528809670126457</v>
-      </c>
-      <c r="L7" s="2"/>
+        <v>1.6384E-4</v>
+      </c>
+      <c r="D10" s="7">
+        <v>2.34305E-4</v>
+      </c>
+      <c r="E10" s="8"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="8"/>
+      <c r="J10" s="7">
+        <v>3.8256400000000001E-4</v>
+      </c>
+      <c r="K10" s="7">
+        <f t="shared" si="2"/>
+        <v>0.61245961460043286</v>
+      </c>
+      <c r="L10" s="7"/>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B8">
-        <v>1048576</v>
-      </c>
-      <c r="C8" s="2">
-        <f t="shared" si="0"/>
-        <v>1.6384E-4</v>
-      </c>
-      <c r="D8" s="2">
-        <v>2.5331799999999999E-4</v>
-      </c>
-      <c r="E8" s="1"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="1"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2">
+    <row r="11" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="6">
+        <v>2097152</v>
+      </c>
+      <c r="C11" s="7">
         <f t="shared" si="1"/>
-        <v>3.8550853077949458</v>
-      </c>
-      <c r="L8" s="2"/>
+        <v>3.2768000000000001E-4</v>
+      </c>
+      <c r="D11" s="7">
+        <v>3.9397500000000002E-4</v>
+      </c>
+      <c r="E11" s="8"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="8"/>
+      <c r="J11" s="7">
+        <v>7.1241200000000005E-4</v>
+      </c>
+      <c r="K11" s="7">
+        <f t="shared" si="2"/>
+        <v>0.55301567070739965</v>
+      </c>
+      <c r="L11" s="7"/>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B9">
-        <v>2097152</v>
-      </c>
-      <c r="C9" s="2">
-        <f t="shared" si="0"/>
-        <v>3.2768000000000001E-4</v>
-      </c>
-      <c r="D9" s="2">
-        <v>4.0695899999999998E-4</v>
-      </c>
-      <c r="E9" s="1"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="1"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2">
+    <row r="12" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="6">
+        <v>4194304</v>
+      </c>
+      <c r="C12" s="7">
         <f t="shared" si="1"/>
-        <v>4.7993163930518801</v>
-      </c>
-      <c r="L9" s="2"/>
+        <v>6.5536000000000001E-4</v>
+      </c>
+      <c r="D12" s="7">
+        <v>6.9665500000000002E-4</v>
+      </c>
+      <c r="E12" s="8"/>
+      <c r="F12" s="7"/>
+      <c r="J12" s="7">
+        <v>1.35732E-3</v>
+      </c>
+      <c r="K12" s="7">
+        <f t="shared" si="2"/>
+        <v>0.51325774319983497</v>
+      </c>
+      <c r="L12" s="7"/>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B10">
-        <v>4194304</v>
-      </c>
-      <c r="C10" s="2">
-        <f t="shared" si="0"/>
-        <v>6.5536000000000001E-4</v>
-      </c>
-      <c r="D10" s="2">
-        <v>7.2393499999999999E-4</v>
-      </c>
-      <c r="E10" s="1"/>
-      <c r="F10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2">
+    <row r="13" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="6">
+        <v>8388608</v>
+      </c>
+      <c r="C13" s="7">
         <f t="shared" si="1"/>
-        <v>5.3958573628847892</v>
-      </c>
-      <c r="L10" s="2"/>
+        <v>1.31072E-3</v>
+      </c>
+      <c r="D13" s="7">
+        <v>1.2886200000000001E-3</v>
+      </c>
+      <c r="E13" s="8"/>
+      <c r="F13" s="7"/>
+      <c r="J13" s="7">
+        <v>2.6243400000000002E-3</v>
+      </c>
+      <c r="K13" s="7">
+        <f t="shared" si="2"/>
+        <v>0.49102631518781864</v>
+      </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B11">
-        <v>8388608</v>
-      </c>
-      <c r="C11" s="2">
-        <f t="shared" si="0"/>
-        <v>1.31072E-3</v>
-      </c>
-      <c r="D11" s="2">
-        <v>1.3516400000000001E-3</v>
-      </c>
-      <c r="E11" s="1"/>
-      <c r="F11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2">
+    <row r="14" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="6">
+        <v>16777216</v>
+      </c>
+      <c r="C14" s="7">
         <f t="shared" si="1"/>
-        <v>5.7800153887129708</v>
-      </c>
-      <c r="L11" s="2"/>
+        <v>2.6214400000000001E-3</v>
+      </c>
+      <c r="D14" s="7">
+        <v>2.3513900000000001E-3</v>
+      </c>
+      <c r="E14" s="8"/>
+      <c r="F14" s="7"/>
+      <c r="J14" s="7">
+        <v>5.6999700000000004E-3</v>
+      </c>
+      <c r="K14" s="7">
+        <f t="shared" si="2"/>
+        <v>0.4125267325968382</v>
+      </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B12">
-        <v>16777216</v>
-      </c>
-      <c r="C12" s="2">
-        <f t="shared" si="0"/>
-        <v>2.6214400000000001E-3</v>
-      </c>
-      <c r="D12" s="2">
-        <v>2.4651600000000001E-3</v>
-      </c>
-      <c r="E12" s="1"/>
-      <c r="F12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2">
-        <f t="shared" si="1"/>
-        <v>6.3383309805448729</v>
-      </c>
-      <c r="L12" s="2"/>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" t="s">
+        <v>50</v>
+      </c>
+      <c r="J16" t="s">
+        <v>0</v>
+      </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="G14" t="s">
-        <v>25</v>
-      </c>
-      <c r="H14" t="s">
-        <v>26</v>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" t="s">
+        <v>53</v>
+      </c>
+      <c r="D17" t="s">
+        <v>51</v>
+      </c>
+      <c r="J17" t="s">
+        <v>54</v>
       </c>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="G15" t="s">
-        <v>28</v>
-      </c>
-      <c r="H15" t="s">
-        <v>27</v>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -4606,11 +6235,400 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC17376B-24CD-2E4E-8489-39C4584887E8}">
+  <dimension ref="A1:L19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="125" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="25.1640625" customWidth="1"/>
+    <col min="3" max="3" width="25.5" customWidth="1"/>
+    <col min="5" max="5" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.83203125" customWidth="1"/>
+    <col min="8" max="8" width="14.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="3">
+        <v>8192</v>
+      </c>
+      <c r="C3" s="4">
+        <f t="shared" ref="C3:C4" si="0">B3/64*10/1000000000</f>
+        <v>1.28E-6</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1.42118E-4</v>
+      </c>
+      <c r="J3" s="5">
+        <v>1.29774E-5</v>
+      </c>
+      <c r="K3" s="4">
+        <f>D3/J3</f>
+        <v>10.951192072371969</v>
+      </c>
+      <c r="L3" s="4"/>
+    </row>
+    <row r="4" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="3">
+        <v>16384</v>
+      </c>
+      <c r="C4" s="4">
+        <f t="shared" si="0"/>
+        <v>2.5600000000000001E-6</v>
+      </c>
+      <c r="D4" s="5">
+        <v>1.04782E-4</v>
+      </c>
+      <c r="J4" s="5">
+        <v>1.5007E-5</v>
+      </c>
+      <c r="K4" s="4">
+        <f t="shared" ref="K4:K14" si="1">D4/J4</f>
+        <v>6.9822083027920305</v>
+      </c>
+      <c r="L4" s="4"/>
+    </row>
+    <row r="5" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="3">
+        <v>32768</v>
+      </c>
+      <c r="C5" s="4">
+        <f t="shared" ref="C5:C14" si="2">B5/64*10/1000000000</f>
+        <v>5.1200000000000001E-6</v>
+      </c>
+      <c r="D5" s="4">
+        <v>1.17465E-4</v>
+      </c>
+      <c r="E5" s="5"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="4">
+        <v>2.0780300000000002E-5</v>
+      </c>
+      <c r="K5" s="4">
+        <f t="shared" si="1"/>
+        <v>5.6527095373984011</v>
+      </c>
+      <c r="L5" s="4"/>
+    </row>
+    <row r="6" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="3">
+        <v>65536</v>
+      </c>
+      <c r="C6" s="4">
+        <f t="shared" si="2"/>
+        <v>1.024E-5</v>
+      </c>
+      <c r="D6" s="4">
+        <v>1.4510400000000001E-4</v>
+      </c>
+      <c r="E6" s="5"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="4">
+        <v>3.5589700000000002E-5</v>
+      </c>
+      <c r="K6" s="4">
+        <f t="shared" si="1"/>
+        <v>4.0771346766058718</v>
+      </c>
+      <c r="L6" s="4"/>
+    </row>
+    <row r="7" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="3">
+        <v>131072</v>
+      </c>
+      <c r="C7" s="4">
+        <f t="shared" si="2"/>
+        <v>2.048E-5</v>
+      </c>
+      <c r="D7" s="4">
+        <v>2.0185900000000001E-4</v>
+      </c>
+      <c r="E7" s="5"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="4">
+        <v>6.3728799999999999E-5</v>
+      </c>
+      <c r="K7" s="4">
+        <f t="shared" si="1"/>
+        <v>3.1674690249934097</v>
+      </c>
+      <c r="L7" s="4"/>
+    </row>
+    <row r="8" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="3">
+        <v>262144</v>
+      </c>
+      <c r="C8" s="4">
+        <f t="shared" si="2"/>
+        <v>4.0960000000000001E-5</v>
+      </c>
+      <c r="D8" s="4">
+        <v>2.1001900000000001E-4</v>
+      </c>
+      <c r="E8" s="5"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="4">
+        <v>1.1654099999999999E-4</v>
+      </c>
+      <c r="K8" s="4">
+        <f t="shared" si="1"/>
+        <v>1.8021039805733605</v>
+      </c>
+      <c r="L8" s="4"/>
+    </row>
+    <row r="9" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="6">
+        <v>524288</v>
+      </c>
+      <c r="C9" s="7">
+        <f t="shared" si="2"/>
+        <v>8.1920000000000002E-5</v>
+      </c>
+      <c r="D9" s="7">
+        <v>2.2035499999999999E-4</v>
+      </c>
+      <c r="E9" s="8"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="8"/>
+      <c r="J9" s="7">
+        <v>2.2104000000000001E-4</v>
+      </c>
+      <c r="K9" s="7">
+        <f t="shared" si="1"/>
+        <v>0.99690101339124126</v>
+      </c>
+      <c r="L9" s="7"/>
+    </row>
+    <row r="10" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="6">
+        <v>1048576</v>
+      </c>
+      <c r="C10" s="7">
+        <f t="shared" si="2"/>
+        <v>1.6384E-4</v>
+      </c>
+      <c r="D10" s="7">
+        <v>3.2559499999999998E-4</v>
+      </c>
+      <c r="E10" s="8"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="8"/>
+      <c r="J10" s="7">
+        <v>4.3998099999999999E-4</v>
+      </c>
+      <c r="K10" s="7">
+        <f t="shared" si="1"/>
+        <v>0.74002059179828217</v>
+      </c>
+      <c r="L10" s="7"/>
+    </row>
+    <row r="11" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="6">
+        <v>2097152</v>
+      </c>
+      <c r="C11" s="7">
+        <f t="shared" si="2"/>
+        <v>3.2768000000000001E-4</v>
+      </c>
+      <c r="D11" s="7">
+        <v>5.6724200000000003E-4</v>
+      </c>
+      <c r="E11" s="8"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="8"/>
+      <c r="J11" s="7">
+        <v>8.5231300000000005E-4</v>
+      </c>
+      <c r="K11" s="7">
+        <f t="shared" si="1"/>
+        <v>0.66553249803769277</v>
+      </c>
+      <c r="L11" s="7"/>
+    </row>
+    <row r="12" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="6">
+        <v>4194304</v>
+      </c>
+      <c r="C12" s="7">
+        <f t="shared" si="2"/>
+        <v>6.5536000000000001E-4</v>
+      </c>
+      <c r="D12" s="7">
+        <v>1.0412799999999999E-3</v>
+      </c>
+      <c r="E12" s="8"/>
+      <c r="F12" s="7"/>
+      <c r="J12" s="7">
+        <v>1.6706799999999999E-3</v>
+      </c>
+      <c r="K12" s="7">
+        <f t="shared" si="1"/>
+        <v>0.62326717264826292</v>
+      </c>
+      <c r="L12" s="7"/>
+    </row>
+    <row r="13" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="6">
+        <v>8388608</v>
+      </c>
+      <c r="C13" s="7">
+        <f t="shared" si="2"/>
+        <v>1.31072E-3</v>
+      </c>
+      <c r="D13" s="7">
+        <v>2.0467100000000002E-3</v>
+      </c>
+      <c r="E13" s="8"/>
+      <c r="F13" s="7"/>
+      <c r="J13" s="7">
+        <v>3.45809E-3</v>
+      </c>
+      <c r="K13" s="7">
+        <f t="shared" si="1"/>
+        <v>0.59186140326018122</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="6">
+        <v>16777216</v>
+      </c>
+      <c r="C14" s="7">
+        <f t="shared" si="2"/>
+        <v>2.6214400000000001E-3</v>
+      </c>
+      <c r="D14" s="7">
+        <v>4.01798E-3</v>
+      </c>
+      <c r="E14" s="8"/>
+      <c r="F14" s="7"/>
+      <c r="J14" s="7">
+        <v>6.8170100000000001E-3</v>
+      </c>
+      <c r="K14" s="7">
+        <f t="shared" si="1"/>
+        <v>0.5894050324115705</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" t="s">
+        <v>50</v>
+      </c>
+      <c r="J16" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" t="s">
+        <v>53</v>
+      </c>
+      <c r="D17" t="s">
+        <v>51</v>
+      </c>
+      <c r="J17" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDFA6D14-5D50-4742-B282-3D26B3553ED8}">
   <dimension ref="A1:P26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="133" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+    <sheetView topLeftCell="A10" zoomScale="139" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5020,10 +7038,10 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="L14" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="M14" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
@@ -5031,21 +7049,21 @@
         <v>9</v>
       </c>
       <c r="M15" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="N15" t="s">
+        <v>26</v>
+      </c>
+      <c r="O15" t="s">
+        <v>27</v>
+      </c>
+      <c r="P15" t="s">
         <v>30</v>
-      </c>
-      <c r="O15" t="s">
-        <v>31</v>
-      </c>
-      <c r="P15" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="K16" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="L16" t="s">
         <v>11</v>
@@ -5057,15 +7075,15 @@
         <v>10</v>
       </c>
       <c r="O16" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="P16" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="P16" s="2" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="17" spans="10:16" x14ac:dyDescent="0.2">
       <c r="K17">
-        <f>B3*10/1024</f>
+        <f t="shared" ref="K17:K26" si="2">B3*10/1024</f>
         <v>320</v>
       </c>
       <c r="L17" s="2">
@@ -5075,21 +7093,21 @@
         <v>7.3958899999999994E-5</v>
       </c>
       <c r="N17" s="2">
-        <f>B3/M17/1024/1024/1024*10</f>
+        <f t="shared" ref="N17:N26" si="3">B3/M17/1024/1024/1024*10</f>
         <v>4.1262888070266062</v>
       </c>
       <c r="O17">
-        <f>K17/16/64</f>
+        <f t="shared" ref="O17:O26" si="4">K17/16/64</f>
         <v>0.3125</v>
       </c>
       <c r="P17" s="2">
-        <f>L17/M17</f>
+        <f t="shared" ref="P17:P26" si="5">L17/M17</f>
         <v>6.6952591236484054</v>
       </c>
     </row>
     <row r="18" spans="10:16" x14ac:dyDescent="0.2">
       <c r="K18">
-        <f>B4*10/1024</f>
+        <f t="shared" si="2"/>
         <v>640</v>
       </c>
       <c r="L18" s="2">
@@ -5099,21 +7117,21 @@
         <v>7.3735700000000006E-5</v>
       </c>
       <c r="N18" s="2">
-        <f>B4/M18/1024/1024/1024*10</f>
+        <f t="shared" si="3"/>
         <v>8.2775583943734166</v>
       </c>
       <c r="O18">
-        <f>K18/16/64</f>
+        <f t="shared" si="4"/>
         <v>0.625</v>
       </c>
       <c r="P18" s="2">
-        <f>L18/M18</f>
+        <f t="shared" si="5"/>
         <v>7.3866254744987829</v>
       </c>
     </row>
     <row r="19" spans="10:16" x14ac:dyDescent="0.2">
       <c r="K19">
-        <f>B5*10/1024</f>
+        <f t="shared" si="2"/>
         <v>1280</v>
       </c>
       <c r="L19" s="2">
@@ -5123,21 +7141,21 @@
         <v>1.4154400000000001E-4</v>
       </c>
       <c r="N19" s="2">
-        <f>B5/M19/1024/1024/1024*10</f>
+        <f t="shared" si="3"/>
         <v>8.6241954798507887</v>
       </c>
       <c r="O19">
-        <f>K19/16/64</f>
+        <f t="shared" si="4"/>
         <v>1.25</v>
       </c>
       <c r="P19" s="2">
-        <f>L19/M19</f>
+        <f t="shared" si="5"/>
         <v>4.273307240151472</v>
       </c>
     </row>
     <row r="20" spans="10:16" x14ac:dyDescent="0.2">
       <c r="K20">
-        <f>B6*10/1024</f>
+        <f t="shared" si="2"/>
         <v>2560</v>
       </c>
       <c r="L20" s="2">
@@ -5147,75 +7165,75 @@
         <v>3.0307100000000003E-4</v>
       </c>
       <c r="N20" s="2">
-        <f>B6/M20/1024/1024/1024*10</f>
+        <f t="shared" si="3"/>
         <v>8.0555587634580679</v>
       </c>
       <c r="O20">
-        <f>K20/16/64</f>
+        <f t="shared" si="4"/>
         <v>2.5</v>
       </c>
       <c r="P20" s="2">
-        <f>L20/M20</f>
+        <f t="shared" si="5"/>
         <v>2.4177535956920986</v>
       </c>
     </row>
     <row r="21" spans="10:16" x14ac:dyDescent="0.2">
-      <c r="J21" t="s">
-        <v>38</v>
-      </c>
-      <c r="K21">
-        <f>B7*10/1024</f>
+      <c r="J21" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="K21" s="9">
+        <f t="shared" si="2"/>
         <v>5120</v>
       </c>
-      <c r="L21" s="2">
+      <c r="L21" s="10">
         <v>1.2528999999999999E-3</v>
       </c>
-      <c r="M21" s="2">
+      <c r="M21" s="10">
         <v>6.9424799999999996E-4</v>
       </c>
-      <c r="N21" s="2">
-        <f>B7/M21/1024/1024/1024*10</f>
+      <c r="N21" s="10">
+        <f t="shared" si="3"/>
         <v>7.0332395628075268</v>
       </c>
-      <c r="O21">
-        <f>K21/16/64</f>
+      <c r="O21" s="9">
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
-      <c r="P21" s="2">
-        <f>L21/M21</f>
+      <c r="P21" s="10">
+        <f t="shared" si="5"/>
         <v>1.8046865097198697</v>
       </c>
     </row>
     <row r="22" spans="10:16" x14ac:dyDescent="0.2">
-      <c r="J22" t="s">
-        <v>37</v>
-      </c>
-      <c r="K22">
-        <f>B8*10/1024</f>
+      <c r="J22" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="K22" s="9">
+        <f t="shared" si="2"/>
         <v>10240</v>
       </c>
-      <c r="L22" s="2">
+      <c r="L22" s="10">
         <v>2.2813500000000001E-3</v>
       </c>
-      <c r="M22" s="2">
+      <c r="M22" s="10">
         <v>1.5307400000000001E-3</v>
       </c>
-      <c r="N22" s="2">
-        <f>B8/M22/1024/1024/1024*10</f>
+      <c r="N22" s="10">
+        <f t="shared" si="3"/>
         <v>6.3796758430562992</v>
       </c>
-      <c r="O22">
-        <f>K22/16/64</f>
+      <c r="O22" s="9">
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
-      <c r="P22" s="2">
-        <f>L22/M22</f>
+      <c r="P22" s="10">
+        <f t="shared" si="5"/>
         <v>1.4903576048185845</v>
       </c>
     </row>
     <row r="23" spans="10:16" x14ac:dyDescent="0.2">
       <c r="K23">
-        <f>B9*10/1024</f>
+        <f t="shared" si="2"/>
         <v>20480</v>
       </c>
       <c r="L23" s="2">
@@ -5225,21 +7243,21 @@
         <v>2.3904600000000001E-3</v>
       </c>
       <c r="N23" s="2">
-        <f>B9/M23/1024/1024/1024*10</f>
+        <f t="shared" si="3"/>
         <v>8.1704985651297228</v>
       </c>
       <c r="O23">
-        <f>K23/16/64</f>
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
       <c r="P23" s="2">
-        <f>L23/M23</f>
+        <f t="shared" si="5"/>
         <v>1.8052174058549402</v>
       </c>
     </row>
     <row r="24" spans="10:16" x14ac:dyDescent="0.2">
       <c r="K24">
-        <f>B10*10/1024</f>
+        <f t="shared" si="2"/>
         <v>40960</v>
       </c>
       <c r="L24" s="2">
@@ -5249,21 +7267,21 @@
         <v>4.8428300000000002E-3</v>
       </c>
       <c r="N24" s="2">
-        <f>B10/M24/1024/1024/1024*10</f>
+        <f t="shared" si="3"/>
         <v>8.066048157792034</v>
       </c>
       <c r="O24">
-        <f>K24/16/64</f>
+        <f t="shared" si="4"/>
         <v>40</v>
       </c>
       <c r="P24" s="2">
-        <f>L24/M24</f>
+        <f t="shared" si="5"/>
         <v>1.6999461058926288</v>
       </c>
     </row>
     <row r="25" spans="10:16" x14ac:dyDescent="0.2">
       <c r="K25">
-        <f>B11*10/1024</f>
+        <f t="shared" si="2"/>
         <v>81920</v>
       </c>
       <c r="L25" s="2">
@@ -5273,24 +7291,24 @@
         <v>9.1571699999999992E-3</v>
       </c>
       <c r="N25" s="2">
-        <f>B11/M25/1024/1024/1024*10</f>
+        <f t="shared" si="3"/>
         <v>8.531565975077454</v>
       </c>
       <c r="O25">
-        <f>K25/16/64</f>
+        <f t="shared" si="4"/>
         <v>80</v>
       </c>
       <c r="P25" s="2">
-        <f>L25/M25</f>
+        <f t="shared" si="5"/>
         <v>1.860771395529405</v>
       </c>
     </row>
     <row r="26" spans="10:16" x14ac:dyDescent="0.2">
       <c r="J26" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="K26">
-        <f>B12*10/1024</f>
+        <f t="shared" si="2"/>
         <v>163840</v>
       </c>
       <c r="L26" s="2">
@@ -5300,15 +7318,15 @@
         <v>2.6890500000000001E-2</v>
       </c>
       <c r="N26" s="2">
-        <f>B12/M26/1024/1024/1024*10</f>
+        <f t="shared" si="3"/>
         <v>5.8106022573027651</v>
       </c>
       <c r="O26">
-        <f>K26/16/64</f>
+        <f t="shared" si="4"/>
         <v>160</v>
       </c>
       <c r="P26" s="2">
-        <f>L26/M26</f>
+        <f t="shared" si="5"/>
         <v>1.0006805377363752</v>
       </c>
     </row>
@@ -5316,4 +7334,106 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AD06957-8614-7941-B63E-DB1F27897B61}">
+  <dimension ref="A3:D10"/>
+  <sheetViews>
+    <sheetView zoomScale="164" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="24.5" customWidth="1"/>
+    <col min="2" max="2" width="75.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1.49386E-5</v>
+      </c>
+      <c r="D6">
+        <v>1.4644699999999999E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="1">
+        <v>3.0174500000000001E-5</v>
+      </c>
+      <c r="D7">
+        <v>1.83122E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="6">
+        <v>1.5266999999999999E-4</v>
+      </c>
+      <c r="D8">
+        <v>1.82781E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="6">
+        <v>2.7673500000000001E-4</v>
+      </c>
+      <c r="D9">
+        <v>2.7345499999999998E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="1">
+        <v>3.03752E-5</v>
+      </c>
+      <c r="D10">
+        <v>1.8627800000000001E-4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
a working version with launch analysis.
</commit_message>
<xml_diff>
--- a/direct_interface_performance.xlsx
+++ b/direct_interface_performance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kanghongbo/Desktop/PIM_at_HW/upmem_communication_performance_test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{262AF9B3-FA59-5F49-871B-F655CCB1DA43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D96CAD50-1528-1B46-9174-C2721C37ACC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5560" yWindow="6860" windowWidth="35080" windowHeight="19240" activeTab="1" xr2:uid="{25B01C09-0A08-DA47-AB65-6825C89D0A76}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" activeTab="3" xr2:uid="{25B01C09-0A08-DA47-AB65-6825C89D0A76}"/>
   </bookViews>
   <sheets>
     <sheet name="Send" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="63">
   <si>
     <t>Direct</t>
   </si>
@@ -205,6 +205,27 @@
   </si>
   <si>
     <t>actual # threads unclear because of UPMEM SDK's implementation</t>
+  </si>
+  <si>
+    <t>dpu_switch_mux_for_rank</t>
+  </si>
+  <si>
+    <t>Components</t>
+  </si>
+  <si>
+    <t>ufi_select_all_even_disabled</t>
+  </si>
+  <si>
+    <t>ufi_set_mram_mux</t>
+  </si>
+  <si>
+    <t>dpu_check_wavegen_mux_status_for_rank</t>
+  </si>
+  <si>
+    <t>1000 rounds * 4 ranks</t>
+  </si>
+  <si>
+    <t>total time</t>
   </si>
 </sst>
 </file>
@@ -6238,7 +6259,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC17376B-24CD-2E4E-8489-39C4584887E8}">
   <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="125" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="125" workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
@@ -7338,24 +7359,27 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AD06957-8614-7941-B63E-DB1F27897B61}">
-  <dimension ref="A3:D10"/>
+  <dimension ref="A3:H22"/>
   <sheetViews>
-    <sheetView zoomScale="164" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="164" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.5" customWidth="1"/>
     <col min="2" max="2" width="75.83203125" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" customWidth="1"/>
+    <col min="5" max="5" width="37" customWidth="1"/>
+    <col min="6" max="17" width="24.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C5" t="s">
         <v>0</v>
       </c>
@@ -7363,7 +7387,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>43</v>
       </c>
@@ -7377,7 +7401,7 @@
         <v>1.4644699999999999E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -7391,7 +7415,7 @@
         <v>1.83122E-4</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>44</v>
       </c>
@@ -7405,7 +7429,7 @@
         <v>1.82781E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>45</v>
       </c>
@@ -7419,7 +7443,7 @@
         <v>2.7345499999999998E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>43</v>
       </c>
@@ -7431,6 +7455,82 @@
       </c>
       <c r="D10">
         <v>1.8627800000000001E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F15" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E16" t="s">
+        <v>57</v>
+      </c>
+      <c r="F16" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="E17" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="E19" t="s">
+        <v>58</v>
+      </c>
+      <c r="F19">
+        <v>8.5353899999999995E-4</v>
+      </c>
+      <c r="G19">
+        <f>F19/4000</f>
+        <v>2.1338474999999999E-7</v>
+      </c>
+      <c r="H19">
+        <f>G19/G22</f>
+        <v>3.1839567069714037E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="E20" t="s">
+        <v>59</v>
+      </c>
+      <c r="F20">
+        <v>4.5667399999999997E-2</v>
+      </c>
+      <c r="G20">
+        <f t="shared" ref="G20:G21" si="0">F20/4000</f>
+        <v>1.1416849999999999E-5</v>
+      </c>
+      <c r="H20">
+        <f>G20/G22</f>
+        <v>0.17035311159764915</v>
+      </c>
+    </row>
+    <row r="21" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="E21" t="s">
+        <v>60</v>
+      </c>
+      <c r="F21">
+        <v>0.221554</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="0"/>
+        <v>5.53885E-5</v>
+      </c>
+      <c r="H21">
+        <f>G21/G22</f>
+        <v>0.82646293169537932</v>
+      </c>
+    </row>
+    <row r="22" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="F22">
+        <f>SUM(F19:F21)</f>
+        <v>0.26807493900000001</v>
+      </c>
+      <c r="G22">
+        <f>SUM(G19:G21)</f>
+        <v>6.7018734750000006E-5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
send working for disabled PIM modules.
</commit_message>
<xml_diff>
--- a/direct_interface_performance.xlsx
+++ b/direct_interface_performance.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kanghongbo/Desktop/PIM_at_HW/upmem_communication_performance_test/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kanghongbo/Desktop/code/upmem_communication_performance_test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D96CAD50-1528-1B46-9174-C2721C37ACC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5156048B-5996-594C-93C8-BE50DD4E12E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" activeTab="3" xr2:uid="{25B01C09-0A08-DA47-AB65-6825C89D0A76}"/>
+    <workbookView xWindow="600" yWindow="1000" windowWidth="33600" windowHeight="18800" activeTab="4" xr2:uid="{25B01C09-0A08-DA47-AB65-6825C89D0A76}"/>
   </bookViews>
   <sheets>
     <sheet name="Send" sheetId="2" r:id="rId1"/>
     <sheet name="Receive" sheetId="3" r:id="rId2"/>
     <sheet name="ReceiveDev" sheetId="1" r:id="rId3"/>
     <sheet name="Launch" sheetId="4" r:id="rId4"/>
+    <sheet name="ParallelResult" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="68">
   <si>
     <t>Direct</t>
   </si>
@@ -227,41 +228,68 @@
   <si>
     <t>total time</t>
   </si>
+  <si>
+    <t>batchsize/MB</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Send Bandwidth</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Default</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Receive Bandwidth</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Light</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.000E+00"/>
+    <numFmt numFmtId="176" formatCode="0.000E+00"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -306,21 +334,21 @@
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="0" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="3" fillId="4" borderId="0" xfId="3" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Bad" xfId="2" builtinId="27"/>
-    <cellStyle name="Good" xfId="1" builtinId="26"/>
-    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="差" xfId="2" builtinId="27"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="好" xfId="1" builtinId="26"/>
+    <cellStyle name="适中" xfId="3" builtinId="28"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -338,7 +366,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="zh-CN"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -400,7 +428,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-CN"/>
+          <a:endParaRPr lang="zh-CN"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -491,7 +519,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-CN"/>
+                  <a:endParaRPr lang="zh-CN"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -807,7 +835,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-CN"/>
+                  <a:endParaRPr lang="zh-CN"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -977,7 +1005,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-CN"/>
+            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1443251776"/>
@@ -1041,7 +1069,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-CN"/>
+            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1443279216"/>
@@ -1083,7 +1111,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-CN"/>
+          <a:endParaRPr lang="zh-CN"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1120,7 +1148,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-CN"/>
+      <a:endParaRPr lang="zh-CN"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1134,7 +1162,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="zh-CN"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1196,7 +1224,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-CN"/>
+          <a:endParaRPr lang="zh-CN"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1287,7 +1315,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-CN"/>
+                  <a:endParaRPr lang="zh-CN"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1603,7 +1631,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-CN"/>
+                  <a:endParaRPr lang="zh-CN"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1773,7 +1801,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-CN"/>
+            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1443251776"/>
@@ -1837,7 +1865,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-CN"/>
+            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1443279216"/>
@@ -1879,7 +1907,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-CN"/>
+          <a:endParaRPr lang="zh-CN"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1916,7 +1944,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-CN"/>
+      <a:endParaRPr lang="zh-CN"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1930,7 +1958,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="zh-CN"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1992,7 +2020,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-CN"/>
+          <a:endParaRPr lang="zh-CN"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2083,7 +2111,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-CN"/>
+                  <a:endParaRPr lang="zh-CN"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -2375,7 +2403,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-CN"/>
+                  <a:endParaRPr lang="zh-CN"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -2533,7 +2561,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-CN"/>
+            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1443251776"/>
@@ -2597,7 +2625,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-CN"/>
+            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1443279216"/>
@@ -2639,7 +2667,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-CN"/>
+          <a:endParaRPr lang="zh-CN"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2676,7 +2704,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-CN"/>
+      <a:endParaRPr lang="zh-CN"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2690,7 +2718,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="zh-CN"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2727,7 +2755,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-CN"/>
+          <a:endParaRPr lang="zh-CN"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3047,7 +3075,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-CN"/>
+            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="939035984"/>
@@ -3111,7 +3139,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-CN"/>
+            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="938787104"/>
@@ -3153,7 +3181,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-CN"/>
+          <a:endParaRPr lang="zh-CN"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3190,7 +3218,1191 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-CN"/>
+      <a:endParaRPr lang="zh-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Send Bandwidth</a:t>
+            </a:r>
+            <a:endParaRPr lang="zh-CN" altLang="zh-CN" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>ParallelResult!$C$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Default</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>ParallelResult!$B$5:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>ParallelResult!$C$5:$C$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>3.2699891857322299</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.6854577711347503</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.637757208054399</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12.625840705423499</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14.6928269716848</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15.9050079892834</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14.9882358949262</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-3890-1A4F-BA7C-68E4A8E9F055}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>ParallelResult!$D$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Light</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>ParallelResult!$B$5:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>ParallelResult!$D$5:$D$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>16.867702061003001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20.269629870904001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22.919429733650102</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>22.481320545748499</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>21.693257745716899</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>19.4119236695925</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>15.0658314409842</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-3890-1A4F-BA7C-68E4A8E9F055}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="761877792"/>
+        <c:axId val="790867712"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="761877792"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-CN" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Batch Size (MB)</a:t>
+                </a:r>
+                <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:sysClr>
+                  </a:solidFill>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="zh-CN"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="790867712"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="790867712"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-CN" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Bandwidth (GB/s)</a:t>
+                </a:r>
+                <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:sysClr>
+                  </a:solidFill>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="zh-CN"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="761877792"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Receive Bandwidth</a:t>
+            </a:r>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>ParallelResult!$C$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Default</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>ParallelResult!$B$15:$B$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>ParallelResult!$C$15:$C$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.70235860529326</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.4342927005091202</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.6898242878346599</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.0322242893175808</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.2635877570816199</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.4427548860244901</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.4320811298319907</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-3E76-B84D-B0D9-31AB3F4C28D3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>ParallelResult!$D$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Light</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>ParallelResult!$B$15:$B$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>ParallelResult!$D$15:$D$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>18.769599601511299</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20.718534537812001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22.400065461231701</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24.503486855131602</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>17.628847936503799</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11.972976065627201</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.8686744283077505</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-3E76-B84D-B0D9-31AB3F4C28D3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="761877792"/>
+        <c:axId val="790867712"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="761877792"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-CN"/>
+                  <a:t>Batch Size (MB)</a:t>
+                </a:r>
+                <a:endParaRPr lang="zh-CN" altLang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="zh-CN"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="790867712"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="790867712"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-CN"/>
+                  <a:t>Bandwidth (GB/s)</a:t>
+                </a:r>
+                <a:endParaRPr lang="zh-CN" altLang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="zh-CN"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="761877792"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-CN"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3361,6 +4573,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -5406,6 +6698,1025 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -5588,8 +7899,87 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>115957</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>71941</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>546653</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>148930</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="图表 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5D14E022-8C40-62C8-C620-37D106F13949}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>728799</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>70994</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>331233</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>147983</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="图表 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{81E6A8CD-BC13-1447-B047-45C6F89C7271}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -5891,7 +8281,7 @@
       <selection activeCell="A16" sqref="A16:J19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="2" max="2" width="18.33203125" customWidth="1"/>
     <col min="3" max="3" width="24.33203125" customWidth="1"/>
@@ -5902,7 +8292,7 @@
     <col min="10" max="10" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12">
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
@@ -5931,7 +8321,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" s="3" customFormat="1">
       <c r="B3" s="3">
         <v>8192</v>
       </c>
@@ -5951,7 +8341,7 @@
       </c>
       <c r="L3" s="4"/>
     </row>
-    <row r="4" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" s="3" customFormat="1">
       <c r="B4" s="3">
         <v>16384</v>
       </c>
@@ -5971,7 +8361,7 @@
       </c>
       <c r="L4" s="4"/>
     </row>
-    <row r="5" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" s="3" customFormat="1">
       <c r="B5" s="3">
         <v>32768</v>
       </c>
@@ -5996,7 +8386,7 @@
       </c>
       <c r="L5" s="4"/>
     </row>
-    <row r="6" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" s="3" customFormat="1">
       <c r="B6" s="3">
         <v>65536</v>
       </c>
@@ -6021,7 +8411,7 @@
       </c>
       <c r="L6" s="4"/>
     </row>
-    <row r="7" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" s="3" customFormat="1">
       <c r="B7" s="3">
         <v>131072</v>
       </c>
@@ -6046,7 +8436,7 @@
       </c>
       <c r="L7" s="4"/>
     </row>
-    <row r="8" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" s="3" customFormat="1">
       <c r="A8" s="3">
         <f>B8/256</f>
         <v>1024</v>
@@ -6075,7 +8465,7 @@
       </c>
       <c r="L8" s="4"/>
     </row>
-    <row r="9" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" s="6" customFormat="1">
       <c r="B9" s="6">
         <v>524288</v>
       </c>
@@ -6098,7 +8488,7 @@
       </c>
       <c r="L9" s="7"/>
     </row>
-    <row r="10" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" s="6" customFormat="1">
       <c r="B10" s="6">
         <v>1048576</v>
       </c>
@@ -6121,7 +8511,7 @@
       </c>
       <c r="L10" s="7"/>
     </row>
-    <row r="11" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" s="6" customFormat="1">
       <c r="B11" s="6">
         <v>2097152</v>
       </c>
@@ -6144,7 +8534,7 @@
       </c>
       <c r="L11" s="7"/>
     </row>
-    <row r="12" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" s="6" customFormat="1">
       <c r="B12" s="6">
         <v>4194304</v>
       </c>
@@ -6166,7 +8556,7 @@
       </c>
       <c r="L12" s="7"/>
     </row>
-    <row r="13" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" s="6" customFormat="1">
       <c r="B13" s="6">
         <v>8388608</v>
       </c>
@@ -6187,7 +8577,7 @@
         <v>0.49102631518781864</v>
       </c>
     </row>
-    <row r="14" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" s="6" customFormat="1">
       <c r="B14" s="6">
         <v>16777216</v>
       </c>
@@ -6208,7 +8598,7 @@
         <v>0.4125267325968382</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -6225,7 +8615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:10">
       <c r="B17" t="s">
         <v>49</v>
       </c>
@@ -6239,17 +8629,18 @@
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:10">
       <c r="B18" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:10">
       <c r="B19" t="s">
         <v>48</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -6263,7 +8654,7 @@
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="2" max="2" width="25.1640625" customWidth="1"/>
     <col min="3" max="3" width="25.5" customWidth="1"/>
@@ -6272,7 +8663,7 @@
     <col min="8" max="8" width="14.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12">
       <c r="B1" t="s">
         <v>21</v>
       </c>
@@ -6292,7 +8683,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12">
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
@@ -6321,7 +8712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" s="3" customFormat="1">
       <c r="B3" s="3">
         <v>8192</v>
       </c>
@@ -6341,7 +8732,7 @@
       </c>
       <c r="L3" s="4"/>
     </row>
-    <row r="4" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" s="3" customFormat="1">
       <c r="B4" s="3">
         <v>16384</v>
       </c>
@@ -6361,7 +8752,7 @@
       </c>
       <c r="L4" s="4"/>
     </row>
-    <row r="5" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" s="3" customFormat="1">
       <c r="B5" s="3">
         <v>32768</v>
       </c>
@@ -6386,7 +8777,7 @@
       </c>
       <c r="L5" s="4"/>
     </row>
-    <row r="6" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" s="3" customFormat="1">
       <c r="B6" s="3">
         <v>65536</v>
       </c>
@@ -6411,7 +8802,7 @@
       </c>
       <c r="L6" s="4"/>
     </row>
-    <row r="7" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" s="3" customFormat="1">
       <c r="B7" s="3">
         <v>131072</v>
       </c>
@@ -6436,7 +8827,7 @@
       </c>
       <c r="L7" s="4"/>
     </row>
-    <row r="8" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" s="3" customFormat="1">
       <c r="B8" s="3">
         <v>262144</v>
       </c>
@@ -6461,7 +8852,7 @@
       </c>
       <c r="L8" s="4"/>
     </row>
-    <row r="9" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" s="6" customFormat="1">
       <c r="B9" s="6">
         <v>524288</v>
       </c>
@@ -6484,7 +8875,7 @@
       </c>
       <c r="L9" s="7"/>
     </row>
-    <row r="10" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" s="6" customFormat="1">
       <c r="B10" s="6">
         <v>1048576</v>
       </c>
@@ -6507,7 +8898,7 @@
       </c>
       <c r="L10" s="7"/>
     </row>
-    <row r="11" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" s="6" customFormat="1">
       <c r="B11" s="6">
         <v>2097152</v>
       </c>
@@ -6530,7 +8921,7 @@
       </c>
       <c r="L11" s="7"/>
     </row>
-    <row r="12" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" s="6" customFormat="1">
       <c r="B12" s="6">
         <v>4194304</v>
       </c>
@@ -6552,7 +8943,7 @@
       </c>
       <c r="L12" s="7"/>
     </row>
-    <row r="13" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" s="6" customFormat="1">
       <c r="B13" s="6">
         <v>8388608</v>
       </c>
@@ -6573,7 +8964,7 @@
         <v>0.59186140326018122</v>
       </c>
     </row>
-    <row r="14" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" s="6" customFormat="1">
       <c r="B14" s="6">
         <v>16777216</v>
       </c>
@@ -6594,7 +8985,7 @@
         <v>0.5894050324115705</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -6611,7 +9002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:10">
       <c r="B17" t="s">
         <v>49</v>
       </c>
@@ -6625,7 +9016,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:10">
       <c r="B18" t="s">
         <v>47</v>
       </c>
@@ -6633,12 +9024,13 @@
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:10">
       <c r="B19" t="s">
         <v>48</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -6652,7 +9044,7 @@
       <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="5" max="5" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.6640625" customWidth="1"/>
@@ -6662,7 +9054,7 @@
     <col min="16" max="16" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -6685,7 +9077,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -6717,7 +9109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16">
       <c r="A3">
         <f>B3/256</f>
         <v>128</v>
@@ -6751,7 +9143,7 @@
         <v>2.2651200000000001E-5</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16">
       <c r="A4">
         <f t="shared" ref="A4:A12" si="1">B4/256</f>
         <v>256</v>
@@ -6785,7 +9177,7 @@
         <v>3.4699700000000003E-5</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16">
       <c r="A5">
         <f t="shared" si="1"/>
         <v>512</v>
@@ -6819,7 +9211,7 @@
         <v>6.2198400000000004E-5</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16">
       <c r="A6">
         <f t="shared" si="1"/>
         <v>1024</v>
@@ -6853,7 +9245,7 @@
         <v>1.17137E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16">
       <c r="A7">
         <f t="shared" si="1"/>
         <v>2048</v>
@@ -6887,7 +9279,7 @@
         <v>2.23465E-4</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16">
       <c r="A8">
         <f t="shared" si="1"/>
         <v>4096</v>
@@ -6921,7 +9313,7 @@
         <v>4.6504000000000001E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16">
       <c r="A9">
         <f t="shared" si="1"/>
         <v>8192</v>
@@ -6955,7 +9347,7 @@
         <v>8.0728799999999997E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16">
       <c r="A10">
         <f t="shared" si="1"/>
         <v>16384</v>
@@ -6989,7 +9381,7 @@
         <v>1.5742600000000001E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16">
       <c r="A11">
         <f t="shared" si="1"/>
         <v>32768</v>
@@ -7023,7 +9415,7 @@
         <v>3.1707100000000002E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16">
       <c r="A12">
         <f t="shared" si="1"/>
         <v>65536</v>
@@ -7057,7 +9449,7 @@
         <v>6.4426500000000003E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16">
       <c r="L14" t="s">
         <v>28</v>
       </c>
@@ -7065,7 +9457,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16">
       <c r="L15" s="2" t="s">
         <v>9</v>
       </c>
@@ -7082,7 +9474,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16">
       <c r="K16" s="2" t="s">
         <v>31</v>
       </c>
@@ -7102,7 +9494,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="10:16" x14ac:dyDescent="0.2">
+    <row r="17" spans="10:16">
       <c r="K17">
         <f t="shared" ref="K17:K26" si="2">B3*10/1024</f>
         <v>320</v>
@@ -7126,7 +9518,7 @@
         <v>6.6952591236484054</v>
       </c>
     </row>
-    <row r="18" spans="10:16" x14ac:dyDescent="0.2">
+    <row r="18" spans="10:16">
       <c r="K18">
         <f t="shared" si="2"/>
         <v>640</v>
@@ -7150,7 +9542,7 @@
         <v>7.3866254744987829</v>
       </c>
     </row>
-    <row r="19" spans="10:16" x14ac:dyDescent="0.2">
+    <row r="19" spans="10:16">
       <c r="K19">
         <f t="shared" si="2"/>
         <v>1280</v>
@@ -7174,7 +9566,7 @@
         <v>4.273307240151472</v>
       </c>
     </row>
-    <row r="20" spans="10:16" x14ac:dyDescent="0.2">
+    <row r="20" spans="10:16">
       <c r="K20">
         <f t="shared" si="2"/>
         <v>2560</v>
@@ -7198,7 +9590,7 @@
         <v>2.4177535956920986</v>
       </c>
     </row>
-    <row r="21" spans="10:16" x14ac:dyDescent="0.2">
+    <row r="21" spans="10:16">
       <c r="J21" s="9" t="s">
         <v>34</v>
       </c>
@@ -7225,7 +9617,7 @@
         <v>1.8046865097198697</v>
       </c>
     </row>
-    <row r="22" spans="10:16" x14ac:dyDescent="0.2">
+    <row r="22" spans="10:16">
       <c r="J22" s="9" t="s">
         <v>33</v>
       </c>
@@ -7252,7 +9644,7 @@
         <v>1.4903576048185845</v>
       </c>
     </row>
-    <row r="23" spans="10:16" x14ac:dyDescent="0.2">
+    <row r="23" spans="10:16">
       <c r="K23">
         <f t="shared" si="2"/>
         <v>20480</v>
@@ -7276,7 +9668,7 @@
         <v>1.8052174058549402</v>
       </c>
     </row>
-    <row r="24" spans="10:16" x14ac:dyDescent="0.2">
+    <row r="24" spans="10:16">
       <c r="K24">
         <f t="shared" si="2"/>
         <v>40960</v>
@@ -7300,7 +9692,7 @@
         <v>1.6999461058926288</v>
       </c>
     </row>
-    <row r="25" spans="10:16" x14ac:dyDescent="0.2">
+    <row r="25" spans="10:16">
       <c r="K25">
         <f t="shared" si="2"/>
         <v>81920</v>
@@ -7324,7 +9716,7 @@
         <v>1.860771395529405</v>
       </c>
     </row>
-    <row r="26" spans="10:16" x14ac:dyDescent="0.2">
+    <row r="26" spans="10:16">
       <c r="J26" t="s">
         <v>35</v>
       </c>
@@ -7352,6 +9744,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -7361,11 +9754,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AD06957-8614-7941-B63E-DB1F27897B61}">
   <dimension ref="A3:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="164" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="164" workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="24.5" customWidth="1"/>
     <col min="2" max="2" width="75.83203125" customWidth="1"/>
@@ -7374,12 +9767,12 @@
     <col min="6" max="17" width="24.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="C5" t="s">
         <v>0</v>
       </c>
@@ -7387,7 +9780,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>43</v>
       </c>
@@ -7401,7 +9794,7 @@
         <v>1.4644699999999999E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -7415,7 +9808,7 @@
         <v>1.83122E-4</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6">
       <c r="A8" s="6" t="s">
         <v>44</v>
       </c>
@@ -7429,7 +9822,7 @@
         <v>1.82781E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6">
       <c r="A9" s="6" t="s">
         <v>45</v>
       </c>
@@ -7443,7 +9836,7 @@
         <v>2.7345499999999998E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>43</v>
       </c>
@@ -7457,12 +9850,12 @@
         <v>1.8627800000000001E-4</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6">
       <c r="F15" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6">
       <c r="E16" t="s">
         <v>57</v>
       </c>
@@ -7470,12 +9863,12 @@
         <v>62</v>
       </c>
     </row>
-    <row r="17" spans="5:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="5:8">
       <c r="E17" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="5:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="5:8">
       <c r="E19" t="s">
         <v>58</v>
       </c>
@@ -7491,7 +9884,7 @@
         <v>3.1839567069714037E-3</v>
       </c>
     </row>
-    <row r="20" spans="5:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="5:8">
       <c r="E20" t="s">
         <v>59</v>
       </c>
@@ -7507,7 +9900,7 @@
         <v>0.17035311159764915</v>
       </c>
     </row>
-    <row r="21" spans="5:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="5:8">
       <c r="E21" t="s">
         <v>60</v>
       </c>
@@ -7523,7 +9916,7 @@
         <v>0.82646293169537932</v>
       </c>
     </row>
-    <row r="22" spans="5:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="5:8">
       <c r="F22">
         <f>SUM(F19:F21)</f>
         <v>0.26807493900000001</v>
@@ -7534,6 +9927,213 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F750D83-0558-B94B-9707-FE6A7D8918D0}">
+  <dimension ref="B3:D21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="179" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="2" max="4" width="18.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:4">
+      <c r="B3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4">
+      <c r="B4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4">
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>3.2699891857322299</v>
+      </c>
+      <c r="D5">
+        <v>16.867702061003001</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4">
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>5.6854577711347503</v>
+      </c>
+      <c r="D6">
+        <v>20.269629870904001</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4">
+      <c r="B7">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>10.637757208054399</v>
+      </c>
+      <c r="D7">
+        <v>22.919429733650102</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4">
+      <c r="B8">
+        <v>16</v>
+      </c>
+      <c r="C8">
+        <v>12.625840705423499</v>
+      </c>
+      <c r="D8">
+        <v>22.481320545748499</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4">
+      <c r="B9">
+        <v>32</v>
+      </c>
+      <c r="C9">
+        <v>14.6928269716848</v>
+      </c>
+      <c r="D9">
+        <v>21.693257745716899</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4">
+      <c r="B10">
+        <v>64</v>
+      </c>
+      <c r="C10">
+        <v>15.9050079892834</v>
+      </c>
+      <c r="D10">
+        <v>19.4119236695925</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4">
+      <c r="B11">
+        <v>128</v>
+      </c>
+      <c r="C11">
+        <v>14.9882358949262</v>
+      </c>
+      <c r="D11">
+        <v>15.0658314409842</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4">
+      <c r="B13" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4">
+      <c r="B14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" t="s">
+        <v>65</v>
+      </c>
+      <c r="D14" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4">
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <v>1.70235860529326</v>
+      </c>
+      <c r="D15">
+        <v>18.769599601511299</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4">
+      <c r="B16">
+        <v>4</v>
+      </c>
+      <c r="C16">
+        <v>3.4342927005091202</v>
+      </c>
+      <c r="D16">
+        <v>20.718534537812001</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4">
+      <c r="B17">
+        <v>8</v>
+      </c>
+      <c r="C17">
+        <v>6.6898242878346599</v>
+      </c>
+      <c r="D17">
+        <v>22.400065461231701</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4">
+      <c r="B18">
+        <v>16</v>
+      </c>
+      <c r="C18">
+        <v>8.0322242893175808</v>
+      </c>
+      <c r="D18">
+        <v>24.503486855131602</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4">
+      <c r="B19">
+        <v>32</v>
+      </c>
+      <c r="C19">
+        <v>8.2635877570816199</v>
+      </c>
+      <c r="D19">
+        <v>17.628847936503799</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4">
+      <c r="B20">
+        <v>64</v>
+      </c>
+      <c r="C20">
+        <v>8.4427548860244901</v>
+      </c>
+      <c r="D20">
+        <v>11.972976065627201</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4">
+      <c r="B21">
+        <v>128</v>
+      </c>
+      <c r="C21">
+        <v>8.4320811298319907</v>
+      </c>
+      <c r="D21">
+        <v>9.8686744283077505</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>